<commit_message>
add code for discretized normal distribution
</commit_message>
<xml_diff>
--- a/survey/loop_fields_dim_10.xlsx
+++ b/survey/loop_fields_dim_10.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinasun/Library/CloudStorage/Dropbox/github_repos/belief_distortion/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C95B16-03E4-464C-B51A-B2B669EDA4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8193CD7-A76C-4049-B49B-2DFCE48417BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4420" yWindow="2060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{98C1675C-38A9-C34E-9946-DFD000C748D0}"/>
   </bookViews>
   <sheets>
     <sheet name="dict" sheetId="1" r:id="rId1"/>
     <sheet name="10x10" sheetId="2" r:id="rId2"/>
+    <sheet name="gen_html_10x10" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Field 1</t>
   </si>
@@ -84,6 +85,9 @@
     <t>Field 11</t>
   </si>
   <si>
+    <t>Field 12</t>
+  </si>
+  <si>
     <t>half position</t>
   </si>
   <si>
@@ -130,6 +134,42 @@
   </si>
   <si>
     <t>mat_b_total_red_loop#</t>
+  </si>
+  <si>
+    <t>treat</t>
+  </si>
+  <si>
+    <t>pairnum</t>
+  </si>
+  <si>
+    <t>halfpos</t>
+  </si>
+  <si>
+    <t>mat_1_half_tag</t>
+  </si>
+  <si>
+    <t>mat_1_whole_tag</t>
+  </si>
+  <si>
+    <t>mat_1_half_red</t>
+  </si>
+  <si>
+    <t>mat_1_total_red</t>
+  </si>
+  <si>
+    <t>mat_2_half_tag</t>
+  </si>
+  <si>
+    <t>mat_2_whole_tag</t>
+  </si>
+  <si>
+    <t>mat_2_half_red</t>
+  </si>
+  <si>
+    <t>mat_2_total_red</t>
+  </si>
+  <si>
+    <t>tasknum</t>
   </si>
 </sst>
 </file>
@@ -490,7 +530,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,13 +580,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -561,45 +601,45 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -610,15 +650,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C203D4-3F67-6347-B273-D2814F4DCD40}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -651,9 +691,70 @@
       </c>
       <c r="K1" t="s">
         <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1379FDFC-C08B-2846-8374-F440DA492F62}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="76.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>